<commit_message>
show the EqualOver specific bid in Winter_16 OFF.
</commit_message>
<xml_diff>
--- a/R-usecases/df_over_under_summary_forslide.xlsx
+++ b/R-usecases/df_over_under_summary_forslide.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="df_over_under_summary_nonewpath" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -61,8 +61,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -550,8 +550,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="20% - Accent1" xfId="22" builtinId="30" customBuiltin="1"/>
@@ -876,10 +876,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="A14:XFD14"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -889,14 +889,17 @@
     <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -913,63 +916,109 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4">
-        <v>-66230789.633286797</v>
+        <v>-80512745.606122807</v>
       </c>
       <c r="C3" s="4">
-        <v>23452675.637922999</v>
+        <v>29065515.726577502</v>
       </c>
       <c r="D3" s="3">
-        <v>13349</v>
+        <v>16366</v>
       </c>
       <c r="E3" s="3">
-        <v>3887</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4545</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4">
-        <v>-15222347.448607501</v>
+        <v>-35545412.737436697</v>
       </c>
       <c r="C4" s="4">
-        <v>35241125.221150599</v>
+        <v>38112052.754308701</v>
       </c>
       <c r="D4" s="3">
-        <v>9187</v>
+        <v>12684</v>
       </c>
       <c r="E4" s="3">
-        <v>5350</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5918</v>
+      </c>
+      <c r="G4" s="4">
+        <f>B4-B$3</f>
+        <v>44967332.86868611</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" ref="H4:J5" si="0">C4-C$3</f>
+        <v>9046537.0277311988</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" si="0"/>
+        <v>-3682</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" si="0"/>
+        <v>1373</v>
+      </c>
+      <c r="K4">
+        <f>G4/H4</f>
+        <v>4.9706680833609065</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4">
-        <v>-17778267.435196199</v>
+        <v>-41092204.375834197</v>
       </c>
       <c r="C5" s="4">
-        <v>34457036.124783002</v>
+        <v>37258708.666714497</v>
       </c>
       <c r="D5" s="3">
-        <v>9543</v>
+        <v>13279</v>
       </c>
       <c r="E5" s="3">
-        <v>5212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5655</v>
+      </c>
+      <c r="G5" s="4">
+        <f t="shared" ref="G5" si="1">B5-B$3</f>
+        <v>39420541.23028861</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="0"/>
+        <v>8193192.9401369952</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="0"/>
+        <v>-3087</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="0"/>
+        <v>1110</v>
+      </c>
+      <c r="K5">
+        <f>G5/H5</f>
+        <v>4.8113771417702598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f>G4/G5</f>
+        <v>1.1407081553242513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -986,63 +1035,63 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="4">
-        <v>-80664202.605393305</v>
+        <v>-80512745.606122807</v>
       </c>
       <c r="C9" s="4">
-        <v>27152025.912954599</v>
+        <v>29065515.726577502</v>
       </c>
       <c r="D9" s="3">
-        <v>16344</v>
+        <v>16366</v>
       </c>
       <c r="E9" s="3">
-        <v>4567</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4545</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="4">
-        <v>-22422445.530878399</v>
+        <v>-35545412.737436697</v>
       </c>
       <c r="C10" s="4">
-        <v>39312378.079080701</v>
+        <v>38112052.754308701</v>
       </c>
       <c r="D10" s="3">
-        <v>11663</v>
+        <v>12684</v>
       </c>
       <c r="E10" s="3">
-        <v>6163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5918</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="4">
-        <v>-25323450.129156899</v>
+        <v>-41092204.375834197</v>
       </c>
       <c r="C11" s="4">
-        <v>38497464.140882596</v>
+        <v>37258708.666714497</v>
       </c>
       <c r="D11" s="3">
-        <v>12033</v>
+        <v>13279</v>
       </c>
       <c r="E11" s="3">
-        <v>6020</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5655</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1059,46 +1108,46 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="4">
         <f>B9-B3</f>
-        <v>-14433412.972106509</v>
+        <v>0</v>
       </c>
       <c r="C15" s="4">
-        <f t="shared" ref="C15:E15" si="0">C9-C3</f>
-        <v>3699350.2750316001</v>
+        <f t="shared" ref="C15:E15" si="2">C9-C3</f>
+        <v>0</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="0"/>
-        <v>2995</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="E15" s="3">
-        <f t="shared" si="0"/>
-        <v>680</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="4">
-        <f t="shared" ref="B16:E16" si="1">B10-B4</f>
-        <v>-7200098.0822708979</v>
+        <f t="shared" ref="B16:E16" si="3">B10-B4</f>
+        <v>0</v>
       </c>
       <c r="C16" s="4">
-        <f t="shared" si="1"/>
-        <v>4071252.8579301015</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="1"/>
-        <v>2476</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="E16" s="3">
-        <f t="shared" si="1"/>
-        <v>813</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1106,82 +1155,82 @@
         <v>2</v>
       </c>
       <c r="B17" s="4">
-        <f t="shared" ref="B17:E17" si="2">B11-B5</f>
-        <v>-7545182.6939607002</v>
+        <f t="shared" ref="B17:E17" si="4">B11-B5</f>
+        <v>0</v>
       </c>
       <c r="C17" s="4">
-        <f t="shared" si="2"/>
-        <v>4040428.0160995945</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="2"/>
-        <v>2490</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="E17" s="3">
-        <f t="shared" si="2"/>
-        <v>808</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="1">
+      <c r="B19" s="1" t="e">
         <f>B16/B15-1</f>
-        <v>-0.50115069137247392</v>
-      </c>
-      <c r="C19" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="C19" s="1" t="e">
         <f>C16/C15-1</f>
-        <v>0.10053186512470069</v>
-      </c>
-      <c r="D19" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="D19" s="1" t="e">
         <f>D16/D15-1</f>
-        <v>-0.17328881469115187</v>
-      </c>
-      <c r="E19" s="1">
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E19" s="1" t="e">
         <f>E16/E15-1</f>
-        <v>0.19558823529411762</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21">
         <f>B16-B$15</f>
-        <v>7233314.889835611</v>
+        <v>0</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:E21" si="3">C16-C$15</f>
-        <v>371902.58289850131</v>
+        <f t="shared" ref="C21:E21" si="5">C16-C$15</f>
+        <v>0</v>
       </c>
       <c r="D21">
-        <f t="shared" si="3"/>
-        <v>-519</v>
+        <f t="shared" si="5"/>
+        <v>0</v>
       </c>
       <c r="E21">
-        <f t="shared" si="3"/>
-        <v>133</v>
-      </c>
-      <c r="G21">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G21" t="e">
         <f>B21/C21</f>
-        <v>19.449488179031306</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22">
-        <f t="shared" ref="B22:E22" si="4">B17-B$15</f>
-        <v>6888230.2781458087</v>
+        <f t="shared" ref="B22:E22" si="6">B17-B$15</f>
+        <v>0</v>
       </c>
       <c r="C22">
-        <f t="shared" si="4"/>
-        <v>341077.74106799439</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="D22">
-        <f t="shared" si="4"/>
-        <v>-505</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="E22">
-        <f t="shared" si="4"/>
-        <v>128</v>
-      </c>
-      <c r="G22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G22" t="e">
         <f>B22/C22</f>
-        <v>20.195484632263437</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>